<commit_message>
added new files to project
</commit_message>
<xml_diff>
--- a/src/main/java/TestData/OrderFormData.xlsx
+++ b/src/main/java/TestData/OrderFormData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\DemoBlazeFramework\src\main\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8ABFA14-EAC3-431C-9DE4-D71B0FA8223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448C6E27-4F53-41A9-AC31-6C625EB17818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1320" windowWidth="22845" windowHeight="6570" xr2:uid="{C7B5716E-0119-442B-9F3B-7C820BDC0121}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{F78567ED-A000-4CEA-A7B1-E88D5FB21C6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>Cape Town</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>2028</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
@@ -119,10 +128,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,17 +446,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34779E1A-9866-4265-893B-EFCE00399973}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC326CC-D36F-4316-846C-C35BF33119F6}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -478,14 +485,14 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2">
-        <v>123456</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2">
-        <v>2028</v>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -496,22 +503,6 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>